<commit_message>
Updated code for table 1
</commit_message>
<xml_diff>
--- a/N uptake/FNRE/FNRE_by_year_Nrate.xlsx
+++ b/N uptake/FNRE/FNRE_by_year_Nrate.xlsx
@@ -411,19 +411,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>76.82892430830945</v>
+        <v>76.82892430830904</v>
       </c>
       <c r="D2">
-        <v>4.441101388449354</v>
+        <v>4.441083924373602</v>
       </c>
       <c r="E2">
-        <v>9.243552439462867</v>
+        <v>7.325201268889618</v>
       </c>
       <c r="F2">
-        <v>66.82266148079545</v>
+        <v>66.42120418721272</v>
       </c>
       <c r="G2">
-        <v>86.83518713582346</v>
+        <v>87.23664442940536</v>
       </c>
       <c r="H2">
         <v>2021</v>
@@ -441,19 +441,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>69.1841244840638</v>
+        <v>69.18412448406353</v>
       </c>
       <c r="D3">
-        <v>4.441101388449353</v>
+        <v>4.44108392437361</v>
       </c>
       <c r="E3">
-        <v>9.243552439462901</v>
+        <v>7.325201268889583</v>
       </c>
       <c r="F3">
-        <v>59.1778616565498</v>
+        <v>58.77640436296718</v>
       </c>
       <c r="G3">
-        <v>79.19038731157781</v>
+        <v>79.59184460515988</v>
       </c>
       <c r="H3">
         <v>2021</v>
@@ -471,19 +471,19 @@
         </is>
       </c>
       <c r="C4">
-        <v>69.95528759880816</v>
+        <v>69.95528759880789</v>
       </c>
       <c r="D4">
-        <v>4.441101388449353</v>
+        <v>4.44108392437361</v>
       </c>
       <c r="E4">
-        <v>9.243552439462906</v>
+        <v>7.325201268889586</v>
       </c>
       <c r="F4">
-        <v>59.94902477129416</v>
+        <v>59.54756747771154</v>
       </c>
       <c r="G4">
-        <v>79.96155042632216</v>
+        <v>80.36300771990423</v>
       </c>
       <c r="H4">
         <v>2021</v>
@@ -501,19 +501,19 @@
         </is>
       </c>
       <c r="C5">
-        <v>66.6763163987666</v>
+        <v>66.67631639876633</v>
       </c>
       <c r="D5">
-        <v>4.441101388449354</v>
+        <v>4.441083924373611</v>
       </c>
       <c r="E5">
-        <v>9.243552439462903</v>
+        <v>7.325201268889577</v>
       </c>
       <c r="F5">
-        <v>56.6700535712526</v>
+        <v>56.26859627766999</v>
       </c>
       <c r="G5">
-        <v>76.68257922628061</v>
+        <v>77.08403651986268</v>
       </c>
       <c r="H5">
         <v>2021</v>
@@ -531,19 +531,19 @@
         </is>
       </c>
       <c r="C6">
-        <v>70.68278148249934</v>
+        <v>70.68278148249907</v>
       </c>
       <c r="D6">
-        <v>4.441101388449353</v>
+        <v>4.441083924373611</v>
       </c>
       <c r="E6">
-        <v>9.243552439462901</v>
+        <v>7.325201268889583</v>
       </c>
       <c r="F6">
-        <v>60.67651865498534</v>
+        <v>60.27506136140272</v>
       </c>
       <c r="G6">
-        <v>80.68904431001334</v>
+        <v>81.09050160359541</v>
       </c>
       <c r="H6">
         <v>2021</v>
@@ -561,19 +561,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>66.0799049127061</v>
+        <v>66.07990491270623</v>
       </c>
       <c r="D7">
-        <v>7.541862354605065</v>
+        <v>7.541864080839908</v>
       </c>
       <c r="E7">
-        <v>13.71467233846437</v>
+        <v>13.71465893073854</v>
       </c>
       <c r="F7">
-        <v>49.87259004198462</v>
+        <v>49.87258481241452</v>
       </c>
       <c r="G7">
-        <v>82.28721978342757</v>
+        <v>82.28722501299794</v>
       </c>
       <c r="H7">
         <v>2022</v>
@@ -591,19 +591,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>52.6725340935274</v>
+        <v>52.67253409352745</v>
       </c>
       <c r="D8">
-        <v>7.541862354605068</v>
+        <v>7.5418640808399</v>
       </c>
       <c r="E8">
-        <v>13.71467233846433</v>
+        <v>13.71465893073853</v>
       </c>
       <c r="F8">
-        <v>36.46521922280591</v>
+        <v>36.46521399323575</v>
       </c>
       <c r="G8">
-        <v>68.87984896424889</v>
+        <v>68.87985419381914</v>
       </c>
       <c r="H8">
         <v>2022</v>
@@ -621,19 +621,19 @@
         </is>
       </c>
       <c r="C9">
-        <v>59.63695759564246</v>
+        <v>59.6369575956425</v>
       </c>
       <c r="D9">
-        <v>7.541862354605069</v>
+        <v>7.5418640808399</v>
       </c>
       <c r="E9">
-        <v>13.71467233846431</v>
+        <v>13.71465893073853</v>
       </c>
       <c r="F9">
-        <v>43.42964272492097</v>
+        <v>43.4296374953508</v>
       </c>
       <c r="G9">
-        <v>75.84427246636395</v>
+        <v>75.8442776959342</v>
       </c>
       <c r="H9">
         <v>2022</v>
@@ -651,19 +651,19 @@
         </is>
       </c>
       <c r="C10">
-        <v>61.6422642741746</v>
+        <v>61.64226427417465</v>
       </c>
       <c r="D10">
-        <v>7.541862354605067</v>
+        <v>7.541864080839901</v>
       </c>
       <c r="E10">
-        <v>13.71467233846433</v>
+        <v>13.71465893073855</v>
       </c>
       <c r="F10">
-        <v>45.43494940345312</v>
+        <v>45.43494417388295</v>
       </c>
       <c r="G10">
-        <v>77.84957914489608</v>
+        <v>77.84958437446635</v>
       </c>
       <c r="H10">
         <v>2022</v>
@@ -681,19 +681,19 @@
         </is>
       </c>
       <c r="C11">
-        <v>65.04838803726237</v>
+        <v>65.04838803726241</v>
       </c>
       <c r="D11">
-        <v>7.541862354605067</v>
+        <v>7.5418640808399</v>
       </c>
       <c r="E11">
-        <v>13.71467233846433</v>
+        <v>13.71465893073856</v>
       </c>
       <c r="F11">
-        <v>48.84107316654089</v>
+        <v>48.84106793697072</v>
       </c>
       <c r="G11">
-        <v>81.25570290798385</v>
+        <v>81.25570813755411</v>
       </c>
       <c r="H11">
         <v>2022</v>
@@ -711,19 +711,19 @@
         </is>
       </c>
       <c r="C12">
-        <v>31.52636143274201</v>
+        <v>31.526361432742</v>
       </c>
       <c r="D12">
-        <v>7.930658819989149</v>
+        <v>7.930658820127168</v>
       </c>
       <c r="E12">
-        <v>20.00000000000034</v>
+        <v>19.99999999999964</v>
       </c>
       <c r="F12">
-        <v>14.98329702150803</v>
+        <v>14.98329702122007</v>
       </c>
       <c r="G12">
-        <v>48.06942584397599</v>
+        <v>48.06942584426392</v>
       </c>
       <c r="H12">
         <v>2023</v>
@@ -744,16 +744,16 @@
         <v>47.88810401080769</v>
       </c>
       <c r="D13">
-        <v>7.930658819989068</v>
+        <v>7.930658820127036</v>
       </c>
       <c r="E13">
-        <v>19.99999999999996</v>
+        <v>20.00000000000002</v>
       </c>
       <c r="F13">
-        <v>31.34503959957386</v>
+        <v>31.34503959928607</v>
       </c>
       <c r="G13">
-        <v>64.43116842204152</v>
+        <v>64.43116842232932</v>
       </c>
       <c r="H13">
         <v>2023</v>
@@ -774,16 +774,16 @@
         <v>53.80783226662075</v>
       </c>
       <c r="D14">
-        <v>7.930658819989072</v>
+        <v>7.930658820127035</v>
       </c>
       <c r="E14">
-        <v>19.99999999999994</v>
+        <v>20.00000000000004</v>
       </c>
       <c r="F14">
-        <v>37.26476785538691</v>
+        <v>37.26476785509912</v>
       </c>
       <c r="G14">
-        <v>70.35089667785459</v>
+        <v>70.35089667814238</v>
       </c>
       <c r="H14">
         <v>2023</v>
@@ -801,19 +801,19 @@
         </is>
       </c>
       <c r="C15">
-        <v>55.65455336500229</v>
+        <v>55.65455336500227</v>
       </c>
       <c r="D15">
-        <v>7.930658819989069</v>
+        <v>7.930658820127036</v>
       </c>
       <c r="E15">
-        <v>19.99999999999996</v>
+        <v>20.00000000000002</v>
       </c>
       <c r="F15">
-        <v>39.11148895376846</v>
+        <v>39.11148895348065</v>
       </c>
       <c r="G15">
-        <v>72.19761777623613</v>
+        <v>72.1976177765239</v>
       </c>
       <c r="H15">
         <v>2023</v>
@@ -831,19 +831,19 @@
         </is>
       </c>
       <c r="C16">
-        <v>56.60476136470481</v>
+        <v>56.60476136470479</v>
       </c>
       <c r="D16">
-        <v>7.930658819989069</v>
+        <v>7.930658820127036</v>
       </c>
       <c r="E16">
-        <v>19.99999999999996</v>
+        <v>20.00000000000002</v>
       </c>
       <c r="F16">
-        <v>40.06169695347097</v>
+        <v>40.06169695318316</v>
       </c>
       <c r="G16">
-        <v>73.14782577593864</v>
+        <v>73.14782577622641</v>
       </c>
       <c r="H16">
         <v>2023</v>
@@ -861,19 +861,19 @@
         </is>
       </c>
       <c r="C17">
-        <v>70.4900422950634</v>
+        <v>70.49004229506329</v>
       </c>
       <c r="D17">
-        <v>4.441101388449357</v>
+        <v>4.441083924373609</v>
       </c>
       <c r="E17">
-        <v>9.243552439462949</v>
+        <v>7.325201268889565</v>
       </c>
       <c r="F17">
-        <v>60.4837794675494</v>
+        <v>60.08232217396694</v>
       </c>
       <c r="G17">
-        <v>80.49630512257741</v>
+        <v>80.89776241615964</v>
       </c>
       <c r="H17">
         <v>2021</v>
@@ -891,19 +891,19 @@
         </is>
       </c>
       <c r="C18">
-        <v>66.97782728910974</v>
+        <v>66.9778272891096</v>
       </c>
       <c r="D18">
-        <v>4.441101388449355</v>
+        <v>4.44108392437361</v>
       </c>
       <c r="E18">
-        <v>9.243552439462949</v>
+        <v>7.32520126888957</v>
       </c>
       <c r="F18">
-        <v>56.97156446159575</v>
+        <v>56.57010716801324</v>
       </c>
       <c r="G18">
-        <v>76.98409011662373</v>
+        <v>77.38554741020596</v>
       </c>
       <c r="H18">
         <v>2021</v>
@@ -921,19 +921,19 @@
         </is>
       </c>
       <c r="C19">
-        <v>70.75056659602001</v>
+        <v>70.75056659601985</v>
       </c>
       <c r="D19">
-        <v>4.441101388449354</v>
+        <v>4.441083924373611</v>
       </c>
       <c r="E19">
-        <v>9.24355243946296</v>
+        <v>7.325201268889561</v>
       </c>
       <c r="F19">
-        <v>60.74430376850601</v>
+        <v>60.34284647492349</v>
       </c>
       <c r="G19">
-        <v>80.756829423534</v>
+        <v>81.15828671711621</v>
       </c>
       <c r="H19">
         <v>2021</v>
@@ -951,19 +951,19 @@
         </is>
       </c>
       <c r="C20">
-        <v>63.60926032708088</v>
+        <v>63.60926032708073</v>
       </c>
       <c r="D20">
-        <v>4.441101388449356</v>
+        <v>4.441083924373611</v>
       </c>
       <c r="E20">
-        <v>9.243552439462958</v>
+        <v>7.325201268889568</v>
       </c>
       <c r="F20">
-        <v>53.60299749956688</v>
+        <v>53.20154020598438</v>
       </c>
       <c r="G20">
-        <v>73.61552315459487</v>
+        <v>74.01698044817709</v>
       </c>
       <c r="H20">
         <v>2021</v>
@@ -981,19 +981,19 @@
         </is>
       </c>
       <c r="C21">
-        <v>62.67615397893913</v>
+        <v>62.67615397893899</v>
       </c>
       <c r="D21">
-        <v>4.441101388449356</v>
+        <v>4.441083924373611</v>
       </c>
       <c r="E21">
-        <v>9.243552439462954</v>
+        <v>7.325201268889573</v>
       </c>
       <c r="F21">
-        <v>52.66989115142514</v>
+        <v>52.26843385784264</v>
       </c>
       <c r="G21">
-        <v>72.68241680645313</v>
+        <v>73.08387410003535</v>
       </c>
       <c r="H21">
         <v>2021</v>
@@ -1011,19 +1011,19 @@
         </is>
       </c>
       <c r="C22">
-        <v>58.92359619305366</v>
+        <v>58.92359619305359</v>
       </c>
       <c r="D22">
-        <v>7.541862354605071</v>
+        <v>7.54186408083991</v>
       </c>
       <c r="E22">
-        <v>13.71467233846431</v>
+        <v>13.71465893073854</v>
       </c>
       <c r="F22">
-        <v>42.71628132233217</v>
+        <v>42.71627609276187</v>
       </c>
       <c r="G22">
-        <v>75.13091106377516</v>
+        <v>75.13091629334531</v>
       </c>
       <c r="H22">
         <v>2022</v>
@@ -1041,19 +1041,19 @@
         </is>
       </c>
       <c r="C23">
-        <v>60.10367771929483</v>
+        <v>60.10367771929485</v>
       </c>
       <c r="D23">
-        <v>7.541862354605072</v>
+        <v>7.541864080839898</v>
       </c>
       <c r="E23">
-        <v>13.71467233846435</v>
+        <v>13.71465893073858</v>
       </c>
       <c r="F23">
-        <v>43.89636284857334</v>
+        <v>43.89635761900317</v>
       </c>
       <c r="G23">
-        <v>76.31099259001633</v>
+        <v>76.31099781958653</v>
       </c>
       <c r="H23">
         <v>2022</v>
@@ -1071,19 +1071,19 @@
         </is>
       </c>
       <c r="C24">
-        <v>66.02944862134746</v>
+        <v>66.02944862134747</v>
       </c>
       <c r="D24">
-        <v>7.541862354605069</v>
+        <v>7.541864080839898</v>
       </c>
       <c r="E24">
-        <v>13.71467233846432</v>
+        <v>13.71465893073854</v>
       </c>
       <c r="F24">
-        <v>49.82213375062597</v>
+        <v>49.82212852105578</v>
       </c>
       <c r="G24">
-        <v>82.23676349206895</v>
+        <v>82.23676872163915</v>
       </c>
       <c r="H24">
         <v>2022</v>
@@ -1101,19 +1101,19 @@
         </is>
       </c>
       <c r="C25">
-        <v>60.40445115423692</v>
+        <v>60.40445115423694</v>
       </c>
       <c r="D25">
-        <v>7.541862354605068</v>
+        <v>7.5418640808399</v>
       </c>
       <c r="E25">
-        <v>13.71467233846433</v>
+        <v>13.71465893073858</v>
       </c>
       <c r="F25">
-        <v>44.19713628351543</v>
+        <v>44.19713105394526</v>
       </c>
       <c r="G25">
-        <v>76.61176602495841</v>
+        <v>76.61177125452862</v>
       </c>
       <c r="H25">
         <v>2022</v>
@@ -1131,19 +1131,19 @@
         </is>
       </c>
       <c r="C26">
-        <v>57.17637533436575</v>
+        <v>57.17637533436577</v>
       </c>
       <c r="D26">
-        <v>7.541862354605068</v>
+        <v>7.5418640808399</v>
       </c>
       <c r="E26">
-        <v>13.71467233846435</v>
+        <v>13.71465893073859</v>
       </c>
       <c r="F26">
-        <v>40.96906046364427</v>
+        <v>40.96905523407408</v>
       </c>
       <c r="G26">
-        <v>73.38369020508723</v>
+        <v>73.38369543465745</v>
       </c>
       <c r="H26">
         <v>2022</v>
@@ -1161,19 +1161,19 @@
         </is>
       </c>
       <c r="C27">
-        <v>52.35291699665521</v>
+        <v>52.35291699665523</v>
       </c>
       <c r="D27">
-        <v>7.93065881998908</v>
+        <v>7.93065882012707</v>
       </c>
       <c r="E27">
-        <v>19.99999999999996</v>
+        <v>20.00000000000002</v>
       </c>
       <c r="F27">
-        <v>35.80985258542135</v>
+        <v>35.80985258513354</v>
       </c>
       <c r="G27">
-        <v>68.89598140788907</v>
+        <v>68.89598140817692</v>
       </c>
       <c r="H27">
         <v>2023</v>
@@ -1191,19 +1191,19 @@
         </is>
       </c>
       <c r="C28">
-        <v>49.62998753730861</v>
+        <v>49.62998753730859</v>
       </c>
       <c r="D28">
-        <v>7.930658819989064</v>
+        <v>7.930658820127032</v>
       </c>
       <c r="E28">
         <v>20.00000000000002</v>
       </c>
       <c r="F28">
-        <v>33.08692312607479</v>
+        <v>33.08692312578698</v>
       </c>
       <c r="G28">
-        <v>66.17305194854242</v>
+        <v>66.17305194883021</v>
       </c>
       <c r="H28">
         <v>2023</v>
@@ -1221,19 +1221,19 @@
         </is>
       </c>
       <c r="C29">
-        <v>55.64881626318222</v>
+        <v>55.64881626318221</v>
       </c>
       <c r="D29">
-        <v>7.930658819989071</v>
+        <v>7.93065882012703</v>
       </c>
       <c r="E29">
-        <v>19.99999999999994</v>
+        <v>20.00000000000007</v>
       </c>
       <c r="F29">
-        <v>39.10575185194838</v>
+        <v>39.1057518516606</v>
       </c>
       <c r="G29">
-        <v>72.19188067441605</v>
+        <v>72.19188067470382</v>
       </c>
       <c r="H29">
         <v>2023</v>
@@ -1254,16 +1254,16 @@
         <v>42.89038706404071</v>
       </c>
       <c r="D30">
-        <v>7.930658819989067</v>
+        <v>7.930658820127022</v>
       </c>
       <c r="E30">
-        <v>20.00000000000002</v>
+        <v>20.00000000000011</v>
       </c>
       <c r="F30">
-        <v>26.34732265280688</v>
+        <v>26.34732265251912</v>
       </c>
       <c r="G30">
-        <v>59.43345147527454</v>
+        <v>59.4334514755623</v>
       </c>
       <c r="H30">
         <v>2023</v>
@@ -1284,16 +1284,16 @@
         <v>50.95037485256204</v>
       </c>
       <c r="D31">
-        <v>7.93065881998907</v>
+        <v>7.930658820127032</v>
       </c>
       <c r="E31">
-        <v>19.99999999999994</v>
+        <v>20.00000000000002</v>
       </c>
       <c r="F31">
-        <v>34.40731044132819</v>
+        <v>34.40731044104042</v>
       </c>
       <c r="G31">
-        <v>67.49343926379588</v>
+        <v>67.49343926408365</v>
       </c>
       <c r="H31">
         <v>2023</v>

</xml_diff>